<commit_message>
Spark - Processo incial de Análise Exploratória
Inicio da praparação dos dataframes para analise exploratoria.
</commit_message>
<xml_diff>
--- a/TabelaEnemAtualizada.xlsx
+++ b/TabelaEnemAtualizada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\GitHub\ProjetoFinalBigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F0E1E9-38CB-40EE-987D-0269F73E6CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7D080-73DC-4048-8CAB-34EB401C80AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3645" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F187853B-A8C3-435C-8CC2-1A1BC972762F}"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="9330" windowHeight="10950" activeTab="1" xr2:uid="{F187853B-A8C3-435C-8CC2-1A1BC972762F}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="312">
   <si>
     <t>[</t>
   </si>
@@ -953,6 +953,15 @@
   </si>
   <si>
     <t>Idade</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -3966,42 +3975,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C51401-3303-4831-B4A8-3C7775A21479}">
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="191" style="1" customWidth="1"/>
-    <col min="3" max="4" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="46.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2015</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>2016</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2017</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2018</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>210</v>
       </c>
@@ -4009,7 +4019,7 @@
         <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>309</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -4023,17 +4033,20 @@
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f>C3</f>
+        <f>D3</f>
         <v xml:space="preserve">'NU_INSCRICAO', </v>
       </c>
       <c r="B3" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
@@ -4047,17 +4060,20 @@
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
-        <f t="shared" ref="A4:A60" si="0">C4</f>
+        <f t="shared" ref="A4:A60" si="0">D4</f>
         <v xml:space="preserve">'NU_ANO', </v>
       </c>
       <c r="B4" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
+      <c r="C4" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -4071,8 +4087,11 @@
       <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'NO_MUNICIPIO_RESIDENCIA', </v>
@@ -4080,8 +4099,8 @@
       <c r="B5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
+      <c r="C5" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -4095,8 +4114,11 @@
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'CO_UF_RESIDENCIA', </v>
@@ -4104,8 +4126,8 @@
       <c r="B6" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -4119,8 +4141,11 @@
       <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'SG_UF_RESIDENCIA',</v>
@@ -4128,8 +4153,8 @@
       <c r="B7" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
+      <c r="C7" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -4143,8 +4168,11 @@
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'NU_IDADE', </v>
@@ -4152,8 +4180,8 @@
       <c r="B8" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
+      <c r="C8" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>17</v>
@@ -4167,8 +4195,11 @@
       <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_SEXO', </v>
@@ -4176,8 +4207,8 @@
       <c r="B9" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
+      <c r="C9" s="6" t="s">
+        <v>310</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -4191,8 +4222,11 @@
       <c r="G9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'TP_ESTADO_CIVIL',</v>
@@ -4200,11 +4234,11 @@
       <c r="B10" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>168</v>
@@ -4215,8 +4249,11 @@
       <c r="G10" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_COR_RACA', </v>
@@ -4224,11 +4261,11 @@
       <c r="B11" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>169</v>
@@ -4239,8 +4276,11 @@
       <c r="G11" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'TP_NACIONALIDADE',</v>
@@ -4248,11 +4288,11 @@
       <c r="B12" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>170</v>
@@ -4263,8 +4303,11 @@
       <c r="G12" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'NO_MUNICIPIO_NASCIMENTO',</v>
@@ -4272,11 +4315,9 @@
       <c r="B13" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>172</v>
@@ -4287,18 +4328,19 @@
       <c r="G13" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
-        <f>C14</f>
+        <f>D14</f>
         <v xml:space="preserve">'CO_UF_NASCIMENTO', </v>
       </c>
       <c r="B14" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
@@ -4311,8 +4353,11 @@
       <c r="G14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'SG_UF_NASCIMENTO', </v>
@@ -4320,11 +4365,9 @@
       <c r="B15" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>173</v>
@@ -4335,8 +4378,11 @@
       <c r="G15" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'TP_ST_CONCLUSAO',</v>
@@ -4344,11 +4390,8 @@
       <c r="B16" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>174</v>
@@ -4359,8 +4402,11 @@
       <c r="G16" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_ESCOLA', </v>
@@ -4368,9 +4414,6 @@
       <c r="B17" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
@@ -4383,8 +4426,11 @@
       <c r="G17" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_ENSINO', </v>
@@ -4392,11 +4438,8 @@
       <c r="B18" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>175</v>
@@ -4407,8 +4450,11 @@
       <c r="G18" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_TREINEIRO', </v>
@@ -4416,9 +4462,6 @@
       <c r="B19" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
@@ -4431,8 +4474,11 @@
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'CO_UF_ESC', </v>
@@ -4440,9 +4486,7 @@
       <c r="B20" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
         <v>12</v>
       </c>
@@ -4455,8 +4499,11 @@
       <c r="G20" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'SG_UF_ESC',</v>
@@ -4464,9 +4511,7 @@
       <c r="B21" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
@@ -4479,8 +4524,11 @@
       <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_DEPENDENCIA_ADM_ESC', </v>
@@ -4488,9 +4536,6 @@
       <c r="B22" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
@@ -4503,8 +4548,11 @@
       <c r="G22" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'TP_LOCALIZACAO_ESC', </v>
@@ -4512,9 +4560,6 @@
       <c r="B23" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
@@ -4527,8 +4572,11 @@
       <c r="G23" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_BAIXA_VISAO', </v>
@@ -4536,9 +4584,6 @@
       <c r="B24" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
@@ -4551,8 +4596,11 @@
       <c r="G24" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_CEGUEIRA', </v>
@@ -4560,9 +4608,6 @@
       <c r="B25" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
@@ -4575,8 +4620,11 @@
       <c r="G25" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_SURDEZ',</v>
@@ -4584,9 +4632,6 @@
       <c r="B26" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
@@ -4599,8 +4644,11 @@
       <c r="G26" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_DEFICIENCIA_AUDITIVA', </v>
@@ -4608,9 +4656,6 @@
       <c r="B27" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
@@ -4623,8 +4668,11 @@
       <c r="G27" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_SURDO_CEGUEIRA',</v>
@@ -4632,9 +4680,6 @@
       <c r="B28" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D28" s="2" t="s">
         <v>34</v>
       </c>
@@ -4647,8 +4692,11 @@
       <c r="G28" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_DEFICIENCIA_FISICA', </v>
@@ -4656,9 +4704,6 @@
       <c r="B29" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D29" s="2" t="s">
         <v>35</v>
       </c>
@@ -4671,8 +4716,11 @@
       <c r="G29" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_DEFICIENCIA_MENTAL',</v>
@@ -4680,9 +4728,6 @@
       <c r="B30" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D30" s="2" t="s">
         <v>36</v>
       </c>
@@ -4695,8 +4740,11 @@
       <c r="G30" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_DEFICIT_ATENCAO', </v>
@@ -4704,9 +4752,6 @@
       <c r="B31" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>37</v>
       </c>
@@ -4719,8 +4764,11 @@
       <c r="G31" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_DISLEXIA', </v>
@@ -4728,9 +4776,6 @@
       <c r="B32" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -4743,8 +4788,11 @@
       <c r="G32" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_DISCALCULIA', </v>
@@ -4752,11 +4800,8 @@
       <c r="B33" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>178</v>
@@ -4767,8 +4812,11 @@
       <c r="G33" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_AUTISMO', </v>
@@ -4776,9 +4824,6 @@
       <c r="B34" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D34" s="2" t="s">
         <v>43</v>
       </c>
@@ -4791,8 +4836,11 @@
       <c r="G34" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_VISAO_MONOCULAR',</v>
@@ -4800,11 +4848,8 @@
       <c r="B35" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>179</v>
@@ -4815,8 +4860,11 @@
       <c r="G35" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_OUTRA_DEF', </v>
@@ -4824,9 +4872,6 @@
       <c r="B36" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D36" s="2" t="s">
         <v>46</v>
       </c>
@@ -4839,8 +4884,11 @@
       <c r="G36" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_GESTANTE', </v>
@@ -4848,14 +4896,11 @@
       <c r="B37" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D37" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>188</v>
@@ -4863,8 +4908,11 @@
       <c r="G37" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_LACTANTE',</v>
@@ -4872,11 +4920,8 @@
       <c r="B38" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>181</v>
@@ -4887,8 +4932,11 @@
       <c r="G38" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_IDOSO', </v>
@@ -4896,14 +4944,11 @@
       <c r="B39" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>41</v>
@@ -4911,8 +4956,11 @@
       <c r="G39" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_ESTUDA_CLASSE_HOSPITALAR', </v>
@@ -4920,14 +4968,11 @@
       <c r="B40" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>189</v>
+        <v>7</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>189</v>
@@ -4935,8 +4980,11 @@
       <c r="G40" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_SEM_RECURSO', </v>
@@ -4944,9 +4992,6 @@
       <c r="B41" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
@@ -4959,8 +5004,11 @@
       <c r="G41" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_BRAILLE', </v>
@@ -4968,14 +5016,11 @@
       <c r="B42" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>49</v>
@@ -4983,8 +5028,11 @@
       <c r="G42" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_AMPLIADA_24', </v>
@@ -4992,9 +5040,6 @@
       <c r="B43" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D43" s="2" t="s">
         <v>50</v>
       </c>
@@ -5007,8 +5052,11 @@
       <c r="G43" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_AMPLIADA_18', </v>
@@ -5016,14 +5064,11 @@
       <c r="B44" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D44" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>190</v>
+        <v>51</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>190</v>
@@ -5031,8 +5076,11 @@
       <c r="G44" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_LEDOR',</v>
@@ -5040,11 +5088,8 @@
       <c r="B45" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>184</v>
@@ -5055,8 +5100,11 @@
       <c r="G45" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_ACESSO', </v>
@@ -5064,14 +5112,11 @@
       <c r="B46" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>53</v>
@@ -5079,8 +5124,11 @@
       <c r="G46" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_TRANSCRICAO', </v>
@@ -5088,9 +5136,6 @@
       <c r="B47" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D47" s="2" t="s">
         <v>54</v>
       </c>
@@ -5103,8 +5148,11 @@
       <c r="G47" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_LIBRAS', </v>
@@ -5112,14 +5160,11 @@
       <c r="B48" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D48" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>191</v>
+        <v>55</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>191</v>
@@ -5127,8 +5172,11 @@
       <c r="G48" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_LEITURA_LABIAL',</v>
@@ -5136,14 +5184,11 @@
       <c r="B49" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D49" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>192</v>
+        <v>56</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>192</v>
@@ -5151,8 +5196,11 @@
       <c r="G49" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_MESA_CADEIRA_RODAS', </v>
@@ -5160,14 +5208,11 @@
       <c r="B50" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="D50" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>193</v>
+        <v>57</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>193</v>
@@ -5175,8 +5220,11 @@
       <c r="G50" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_MESA_CADEIRA_SEPARADA',</v>
@@ -5184,14 +5232,11 @@
       <c r="B51" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D51" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>194</v>
+        <v>58</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>194</v>
@@ -5199,8 +5244,11 @@
       <c r="G51" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_APOIO_PERNA', </v>
@@ -5208,9 +5256,6 @@
       <c r="B52" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="D52" s="2" t="s">
         <v>59</v>
       </c>
@@ -5223,8 +5268,11 @@
       <c r="G52" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_GUIA_INTERPRETE', </v>
@@ -5232,14 +5280,11 @@
       <c r="B53" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D53" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>195</v>
+        <v>60</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>195</v>
@@ -5247,8 +5292,11 @@
       <c r="G53" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_COMPUTADOR',</v>
@@ -5256,14 +5304,11 @@
       <c r="B54" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D54" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>196</v>
+        <v>62</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>196</v>
@@ -5271,8 +5316,11 @@
       <c r="G54" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_CADEIRA_ESPECIAL', </v>
@@ -5280,9 +5328,6 @@
       <c r="B55" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="D55" s="2" t="s">
         <v>63</v>
       </c>
@@ -5295,8 +5340,11 @@
       <c r="G55" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_CADEIRA_CANHOTO',</v>
@@ -5304,9 +5352,6 @@
       <c r="B56" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D56" s="2" t="s">
         <v>64</v>
       </c>
@@ -5319,8 +5364,11 @@
       <c r="G56" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_CADEIRA_ACOLCHOADA', </v>
@@ -5328,9 +5376,6 @@
       <c r="B57" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D57" s="2" t="s">
         <v>65</v>
       </c>
@@ -5343,8 +5388,11 @@
       <c r="G57" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_PROVA_DEITADO', </v>
@@ -5352,9 +5400,6 @@
       <c r="B58" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D58" s="2" t="s">
         <v>66</v>
       </c>
@@ -5367,8 +5412,11 @@
       <c r="G58" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'IN_MOBILIARIO_OBESO',</v>
@@ -5376,9 +5424,6 @@
       <c r="B59" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D59" s="2" t="s">
         <v>67</v>
       </c>
@@ -5391,8 +5436,11 @@
       <c r="G59" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">'IN_LAMINA_OVERLAY', </v>
@@ -5400,9 +5448,6 @@
       <c r="B60" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D60" s="2" t="s">
         <v>68</v>
       </c>
@@ -5415,18 +5460,18 @@
       <c r="G60" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="str">
-        <f t="shared" ref="A61:A92" si="1">C61</f>
+        <f t="shared" ref="A61:A92" si="1">D61</f>
         <v xml:space="preserve">'IN_PROTETOR_AURICULAR', </v>
       </c>
       <c r="B61" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D61" s="2" t="s">
         <v>69</v>
       </c>
@@ -5439,8 +5484,11 @@
       <c r="G61" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'IN_MEDIDOR_GLICOSE',</v>
@@ -5448,9 +5496,6 @@
       <c r="B62" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D62" s="2" t="s">
         <v>70</v>
       </c>
@@ -5463,8 +5508,11 @@
       <c r="G62" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_MAQUINA_BRAILE', </v>
@@ -5472,9 +5520,6 @@
       <c r="B63" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D63" s="2" t="s">
         <v>71</v>
       </c>
@@ -5487,8 +5532,11 @@
       <c r="G63" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_SOROBAN', </v>
@@ -5496,9 +5544,6 @@
       <c r="B64" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D64" s="2" t="s">
         <v>72</v>
       </c>
@@ -5511,8 +5556,11 @@
       <c r="G64" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_MARCA_PASSO', </v>
@@ -5520,9 +5568,6 @@
       <c r="B65" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D65" s="2" t="s">
         <v>73</v>
       </c>
@@ -5535,8 +5580,11 @@
       <c r="G65" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'IN_SONDA',</v>
@@ -5544,9 +5592,6 @@
       <c r="B66" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D66" s="2" t="s">
         <v>74</v>
       </c>
@@ -5559,8 +5604,11 @@
       <c r="G66" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_MEDICAMENTOS', </v>
@@ -5568,9 +5616,6 @@
       <c r="B67" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D67" s="2" t="s">
         <v>75</v>
       </c>
@@ -5583,8 +5628,11 @@
       <c r="G67" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_SALA_INDIVIDUAL', </v>
@@ -5592,9 +5640,6 @@
       <c r="B68" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D68" s="2" t="s">
         <v>76</v>
       </c>
@@ -5607,8 +5652,11 @@
       <c r="G68" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'IN_SALA_ESPECIAL',</v>
@@ -5616,9 +5664,6 @@
       <c r="B69" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D69" s="2" t="s">
         <v>77</v>
       </c>
@@ -5631,8 +5676,11 @@
       <c r="G69" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_SALA_ACOMPANHANTE', </v>
@@ -5640,9 +5688,6 @@
       <c r="B70" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D70" s="2" t="s">
         <v>78</v>
       </c>
@@ -5655,8 +5700,11 @@
       <c r="G70" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'IN_MOBILIARIO_ESPECIFICO',</v>
@@ -5664,9 +5712,6 @@
       <c r="B71" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="D71" s="2" t="s">
         <v>79</v>
       </c>
@@ -5679,8 +5724,11 @@
       <c r="G71" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'IN_MATERIAL_ESPECÍFICO', </v>
@@ -5688,11 +5736,8 @@
       <c r="B72" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>186</v>
@@ -5703,8 +5748,11 @@
       <c r="G72" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'IN_NOME_SOCIAL',</v>
@@ -5712,11 +5760,8 @@
       <c r="B73" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>187</v>
@@ -5727,8 +5772,11 @@
       <c r="G73" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NO_MUNICIPIO_PROVA', </v>
@@ -5736,9 +5784,6 @@
       <c r="B74" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D74" s="2" t="s">
         <v>86</v>
       </c>
@@ -5751,8 +5796,11 @@
       <c r="G74" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'CO_UF_PROVA', </v>
@@ -5760,9 +5808,7 @@
       <c r="B75" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="C75" s="4"/>
       <c r="D75" s="2" t="s">
         <v>87</v>
       </c>
@@ -5775,8 +5821,11 @@
       <c r="G75" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'SG_UF_PROVA',</v>
@@ -5784,9 +5833,7 @@
       <c r="B76" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="2" t="s">
         <v>88</v>
       </c>
@@ -5799,8 +5846,11 @@
       <c r="G76" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'TP_PRESENCA_CN', </v>
@@ -5808,9 +5858,6 @@
       <c r="B77" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D77" s="2" t="s">
         <v>89</v>
       </c>
@@ -5823,8 +5870,11 @@
       <c r="G77" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'TP_PRESENCA_CH', </v>
@@ -5832,9 +5882,6 @@
       <c r="B78" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="D78" s="2" t="s">
         <v>90</v>
       </c>
@@ -5847,8 +5894,11 @@
       <c r="G78" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'TP_PRESENCA_LC',</v>
@@ -5856,9 +5906,6 @@
       <c r="B79" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D79" s="2" t="s">
         <v>91</v>
       </c>
@@ -5871,8 +5918,11 @@
       <c r="G79" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'TP_PRESENCA_MT', </v>
@@ -5880,9 +5930,6 @@
       <c r="B80" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D80" s="2" t="s">
         <v>92</v>
       </c>
@@ -5895,8 +5942,11 @@
       <c r="G80" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_CN', </v>
@@ -5904,9 +5954,7 @@
       <c r="B81" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="C81" s="4"/>
       <c r="D81" s="2" t="s">
         <v>97</v>
       </c>
@@ -5919,8 +5967,11 @@
       <c r="G81" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_CH', </v>
@@ -5928,9 +5979,7 @@
       <c r="B82" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="C82" s="4"/>
       <c r="D82" s="2" t="s">
         <v>98</v>
       </c>
@@ -5943,8 +5992,11 @@
       <c r="G82" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'NU_NOTA_LC',</v>
@@ -5952,9 +6004,7 @@
       <c r="B83" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C83" s="4"/>
       <c r="D83" s="2" t="s">
         <v>99</v>
       </c>
@@ -5967,8 +6017,11 @@
       <c r="G83" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_MT', </v>
@@ -5976,9 +6029,7 @@
       <c r="B84" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="C84" s="4"/>
       <c r="D84" s="2" t="s">
         <v>100</v>
       </c>
@@ -5991,8 +6042,11 @@
       <c r="G84" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'TP_LINGUA',</v>
@@ -6000,9 +6054,6 @@
       <c r="B85" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D85" s="2" t="s">
         <v>105</v>
       </c>
@@ -6015,8 +6066,11 @@
       <c r="G85" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'TP_STATUS_REDACAO', </v>
@@ -6024,9 +6078,6 @@
       <c r="B86" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D86" s="2" t="s">
         <v>110</v>
       </c>
@@ -6039,8 +6090,11 @@
       <c r="G86" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'NU_NOTA_COMP1',</v>
@@ -6048,9 +6102,7 @@
       <c r="B87" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="C87" s="7"/>
       <c r="D87" s="2" t="s">
         <v>111</v>
       </c>
@@ -6063,8 +6115,11 @@
       <c r="G87" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_COMP2', </v>
@@ -6072,9 +6127,7 @@
       <c r="B88" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="C88" s="7"/>
       <c r="D88" s="2" t="s">
         <v>112</v>
       </c>
@@ -6087,8 +6140,11 @@
       <c r="G88" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_COMP3', </v>
@@ -6096,9 +6152,7 @@
       <c r="B89" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="C89" s="7"/>
       <c r="D89" s="2" t="s">
         <v>113</v>
       </c>
@@ -6111,8 +6165,11 @@
       <c r="G89" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_COMP4', </v>
@@ -6120,9 +6177,7 @@
       <c r="B90" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="C90" s="7"/>
       <c r="D90" s="2" t="s">
         <v>114</v>
       </c>
@@ -6135,8 +6190,11 @@
       <c r="G90" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>'NU_NOTA_COMP5',</v>
@@ -6144,9 +6202,7 @@
       <c r="B91" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="C91" s="7"/>
       <c r="D91" s="2" t="s">
         <v>115</v>
       </c>
@@ -6159,8 +6215,11 @@
       <c r="G91" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">'NU_NOTA_REDACAO', </v>
@@ -6168,9 +6227,7 @@
       <c r="B92" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="C92" s="4"/>
       <c r="D92" s="2" t="s">
         <v>116</v>
       </c>
@@ -6183,17 +6240,18 @@
       <c r="G92" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
         <v>117</v>
       </c>
@@ -6206,17 +6264,18 @@
       <c r="G93" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
         <v>118</v>
       </c>
@@ -6229,17 +6288,18 @@
       <c r="G94" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>121</v>
-      </c>
+      <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
         <v>121</v>
       </c>
@@ -6252,17 +6312,18 @@
       <c r="G95" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>122</v>
       </c>
@@ -6275,17 +6336,18 @@
       <c r="G96" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
         <v>138</v>
       </c>
@@ -6298,17 +6360,18 @@
       <c r="G97" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
         <v>140</v>
       </c>
@@ -6321,17 +6384,18 @@
       <c r="G98" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>199</v>
-      </c>
+      <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
         <v>199</v>
       </c>
@@ -6344,11 +6408,11 @@
       <c r="G99" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C100" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="H99" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D100" s="1" t="s">
         <v>167</v>
       </c>
@@ -6361,235 +6425,235 @@
       <c r="G100" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="1" t="s">
+      <c r="H100" s="1" t="s">
         <v>167</v>
       </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="1" t="s">
+      <c r="E117" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C119" s="1" t="s">
-        <v>61</v>
-      </c>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C120" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="E119" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C121" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="E120" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C122" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="E121" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C123" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="E122" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C124" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="E123" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C125" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="E124" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C126" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="E125" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C127" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="E126" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C128" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="E127" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D128" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C129" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="E128" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D129" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C130" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="E129" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D130" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="E130" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="1" t="s">
-        <v>128</v>
-      </c>
+    <row r="131" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D131" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C132" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="E131" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D132" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C133" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="E132" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D133" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C134" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="E133" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D134" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C135" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="E134" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D135" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C136" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="E135" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D136" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C137" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="E136" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D137" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C138" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="E137" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="138" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D138" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C139" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="E138" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D139" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C140" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="E139" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="140" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D140" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C141" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="E140" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="141" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D141" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="E141" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D142" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C143" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="E142" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D143" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="1" t="s">
-        <v>144</v>
-      </c>
+      <c r="E143" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D144" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>119</v>
@@ -6597,16 +6661,16 @@
       <c r="G144" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C145" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="H144" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="145" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D145" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>120</v>
@@ -6614,16 +6678,16 @@
       <c r="G145" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C146" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="H145" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="146" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D146" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>123</v>
@@ -6631,16 +6695,16 @@
       <c r="G146" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C147" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="H146" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="147" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D147" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>124</v>
@@ -6648,16 +6712,16 @@
       <c r="G147" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C148" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="H147" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="148" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D148" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>125</v>
@@ -6665,16 +6729,16 @@
       <c r="G148" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C149" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="H148" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D149" s="1" t="s">
         <v>149</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>126</v>
@@ -6682,16 +6746,16 @@
       <c r="G149" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C150" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="H149" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="150" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D150" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>127</v>
@@ -6699,16 +6763,16 @@
       <c r="G150" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C151" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="H150" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="151" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D151" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>128</v>
@@ -6716,16 +6780,16 @@
       <c r="G151" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="152" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C152" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="H151" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="152" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D152" s="1" t="s">
         <v>152</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>129</v>
@@ -6733,16 +6797,16 @@
       <c r="G152" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="153" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C153" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="H152" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="153" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D153" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>130</v>
@@ -6750,16 +6814,16 @@
       <c r="G153" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="154" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C154" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="H153" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="154" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D154" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>131</v>
@@ -6767,16 +6831,16 @@
       <c r="G154" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="155" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C155" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="H154" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="155" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D155" s="1" t="s">
         <v>155</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>132</v>
@@ -6784,16 +6848,16 @@
       <c r="G155" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="156" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C156" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="H155" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="156" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D156" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>133</v>
@@ -6801,16 +6865,16 @@
       <c r="G156" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="157" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C157" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="H156" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D157" s="1" t="s">
         <v>157</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>134</v>
@@ -6818,16 +6882,16 @@
       <c r="G157" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C158" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="H157" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="158" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D158" s="1" t="s">
         <v>158</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>135</v>
@@ -6835,16 +6899,16 @@
       <c r="G158" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C159" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="H158" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="159" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D159" s="1" t="s">
         <v>159</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>136</v>
@@ -6852,16 +6916,16 @@
       <c r="G159" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="160" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C160" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="H159" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="160" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D160" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>137</v>
@@ -6869,16 +6933,16 @@
       <c r="G160" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C161" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="H160" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D161" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>139</v>
@@ -6886,35 +6950,35 @@
       <c r="G161" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C162" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="H161" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D162" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C163" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="E162" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D163" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C164" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="E163" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D164" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C165" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="E164" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D165" s="2" t="s">
         <v>25</v>
       </c>
@@ -6927,13 +6991,13 @@
       <c r="G165" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C166" s="2" t="s">
+      <c r="H165" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D166" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>176</v>
@@ -6944,13 +7008,13 @@
       <c r="G166" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C167" s="2" t="s">
+      <c r="H166" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D167" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>177</v>
@@ -6961,11 +7025,11 @@
       <c r="G167" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C168" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="H167" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D168" s="2" t="s">
         <v>11</v>
       </c>
@@ -6978,11 +7042,11 @@
       <c r="G168" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C169" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="H168" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D169" s="2" t="s">
         <v>16</v>
       </c>
@@ -6995,11 +7059,11 @@
       <c r="G169" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C170" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="H169" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D170" s="2" t="s">
         <v>93</v>
       </c>
@@ -7012,11 +7076,11 @@
       <c r="G170" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C171" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="H170" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D171" s="2" t="s">
         <v>94</v>
       </c>
@@ -7029,11 +7093,11 @@
       <c r="G171" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C172" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="H171" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D172" s="2" t="s">
         <v>95</v>
       </c>
@@ -7046,11 +7110,11 @@
       <c r="G172" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C173" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="H172" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D173" s="2" t="s">
         <v>96</v>
       </c>
@@ -7063,14 +7127,14 @@
       <c r="G173" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H173" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="str">
-        <f t="shared" ref="A174:A181" si="2">C174</f>
+        <f t="shared" ref="A174:A181" si="2">D174</f>
         <v xml:space="preserve">'TX_RESPOSTAS_CN', </v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>101</v>
@@ -7084,15 +7148,15 @@
       <c r="G174" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H174" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="str">
         <f t="shared" si="2"/>
         <v>'TX_RESPOSTAS_CH',</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="D175" s="2" t="s">
         <v>102</v>
       </c>
@@ -7105,15 +7169,15 @@
       <c r="G175" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H175" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">'TX_RESPOSTAS_LC', </v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="D176" s="2" t="s">
         <v>103</v>
       </c>
@@ -7126,15 +7190,15 @@
       <c r="G176" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H176" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">'TX_RESPOSTAS_MT', </v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="D177" s="2" t="s">
         <v>104</v>
       </c>
@@ -7147,15 +7211,15 @@
       <c r="G177" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H177" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">'TX_GABARITO_CN', </v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="D178" s="2" t="s">
         <v>106</v>
       </c>
@@ -7168,15 +7232,15 @@
       <c r="G178" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H178" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">'TX_GABARITO_CH', </v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D179" s="2" t="s">
         <v>107</v>
       </c>
@@ -7189,15 +7253,15 @@
       <c r="G179" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H179" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="str">
         <f t="shared" si="2"/>
         <v>'TX_GABARITO_LC',</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="D180" s="2" t="s">
         <v>108</v>
       </c>
@@ -7210,15 +7274,15 @@
       <c r="G180" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H180" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">'TX_GABARITO_MT', </v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="D181" s="2" t="s">
         <v>109</v>
       </c>
@@ -7231,51 +7295,51 @@
       <c r="G181" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H181" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C182" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D182" s="3" t="s">
         <v>162</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G182" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C183" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D183" s="3" t="s">
         <v>163</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="G183" s="1" t="s">
+      <c r="G183" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H183" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="str">
-        <f>C184</f>
+        <f>D184</f>
         <v>'CO_MUNICIPIO_RESIDENCIA',</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>3</v>
@@ -7289,18 +7353,19 @@
       <c r="G184" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H184" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="str">
-        <f>C185</f>
+        <f>D185</f>
         <v xml:space="preserve">'CO_MUNICIPIO_NASCIMENTO', </v>
       </c>
       <c r="B185" s="6"/>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="6"/>
+      <c r="D185" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="E185" s="2" t="s">
         <v>171</v>
@@ -7311,14 +7376,14 @@
       <c r="G185" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H185" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="str">
-        <f>C186</f>
+        <f>D186</f>
         <v>'CO_MUNICIPIO_PROVA',</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>85</v>
@@ -7330,6 +7395,9 @@
         <v>85</v>
       </c>
       <c r="G186" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H186" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Criação Notebook com Spark
Criação do Notebook do Projeto Final, com o framework Spark e início da análise exploratória.
</commit_message>
<xml_diff>
--- a/TabelaEnemAtualizada.xlsx
+++ b/TabelaEnemAtualizada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\GitHub\ProjetoFinalBigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7D080-73DC-4048-8CAB-34EB401C80AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B45FA3-9825-43DB-B4D5-A3595A995675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="30" windowWidth="9330" windowHeight="10950" activeTab="1" xr2:uid="{F187853B-A8C3-435C-8CC2-1A1BC972762F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F187853B-A8C3-435C-8CC2-1A1BC972762F}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="309">
   <si>
     <t>[</t>
   </si>
@@ -868,9 +868,6 @@
     <t>Indicador de solicitação de mobiliário específico</t>
   </si>
   <si>
-    <t>Indicador de solicitação de material específico</t>
-  </si>
-  <si>
     <t>Indicador de inscrito que se declarou travesti, transexual ou transgênero e solicitou atendimento pelo Nome Social, conforme é reconhecido socialmente em consonância com sua identidade de gênero</t>
   </si>
   <si>
@@ -956,12 +953,6 @@
   </si>
   <si>
     <t>TIPO</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -3975,10 +3966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C51401-3303-4831-B4A8-3C7775A21479}">
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4019,7 +4010,7 @@
         <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -4045,9 +4036,6 @@
       <c r="B3" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -4072,9 +4060,7 @@
       <c r="B4" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>310</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -4099,9 +4085,7 @@
       <c r="B5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>310</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
@@ -4126,9 +4110,7 @@
       <c r="B6" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>311</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
@@ -4153,9 +4135,7 @@
       <c r="B7" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>310</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
@@ -4178,11 +4158,9 @@
         <v xml:space="preserve">'NU_IDADE', </v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>310</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
@@ -4207,9 +4185,7 @@
       <c r="B9" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
@@ -4234,9 +4210,7 @@
       <c r="B10" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
@@ -4261,9 +4235,7 @@
       <c r="B11" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
@@ -4288,9 +4260,7 @@
       <c r="B12" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
@@ -5466,7 +5436,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="str">
-        <f t="shared" ref="A61:A92" si="1">D61</f>
+        <f t="shared" ref="A61:A91" si="1">D61</f>
         <v xml:space="preserve">'IN_PROTETOR_AURICULAR', </v>
       </c>
       <c r="B61" s="1" t="s">
@@ -5731,1673 +5701,1649 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'IN_MATERIAL_ESPECÍFICO', </v>
+        <v>'IN_NOME_SOCIAL',</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>280</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'IN_NOME_SOCIAL',</v>
+        <v xml:space="preserve">'NO_MUNICIPIO_PROVA', </v>
       </c>
       <c r="B73" s="1" t="s">
         <v>281</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>187</v>
+        <v>86</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>187</v>
+        <v>86</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>187</v>
+        <v>86</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NO_MUNICIPIO_PROVA', </v>
-      </c>
-      <c r="B74" s="1" t="s">
+        <v xml:space="preserve">'CO_UF_PROVA', </v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>282</v>
       </c>
+      <c r="C74" s="4"/>
       <c r="D74" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'CO_UF_PROVA', </v>
+        <v>'SG_UF_PROVA',</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'SG_UF_PROVA',</v>
-      </c>
-      <c r="B76" s="4" t="s">
+        <v xml:space="preserve">'TP_PRESENCA_CN', </v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C76" s="4"/>
       <c r="D76" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'TP_PRESENCA_CN', </v>
+        <v xml:space="preserve">'TP_PRESENCA_CH', </v>
       </c>
       <c r="B77" s="1" t="s">
         <v>285</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'TP_PRESENCA_CH', </v>
+        <v>'TP_PRESENCA_LC',</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>286</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'TP_PRESENCA_LC',</v>
+        <v xml:space="preserve">'TP_PRESENCA_MT', </v>
       </c>
       <c r="B79" s="1" t="s">
         <v>287</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'TP_PRESENCA_MT', </v>
-      </c>
-      <c r="B80" s="1" t="s">
+        <v xml:space="preserve">'NU_NOTA_CN', </v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>288</v>
       </c>
+      <c r="C80" s="4"/>
       <c r="D80" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_CN', </v>
+        <v xml:space="preserve">'NU_NOTA_CH', </v>
       </c>
       <c r="B81" s="4" t="s">
         <v>289</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_CH', </v>
+        <v>'NU_NOTA_LC',</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>290</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'NU_NOTA_LC',</v>
+        <v xml:space="preserve">'NU_NOTA_MT', </v>
       </c>
       <c r="B83" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_MT', </v>
-      </c>
-      <c r="B84" s="4" t="s">
+        <v>'TP_LINGUA',</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C84" s="4"/>
       <c r="D84" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'TP_LINGUA',</v>
+        <v xml:space="preserve">'TP_STATUS_REDACAO', </v>
       </c>
       <c r="B85" s="1" t="s">
         <v>293</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'TP_STATUS_REDACAO', </v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>294</v>
-      </c>
+        <v>'NU_NOTA_COMP1',</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C86" s="7"/>
       <c r="D86" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'NU_NOTA_COMP1',</v>
+        <v xml:space="preserve">'NU_NOTA_COMP2', </v>
       </c>
       <c r="B87" s="7" t="s">
         <v>303</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_COMP2', </v>
+        <v xml:space="preserve">'NU_NOTA_COMP3', </v>
       </c>
       <c r="B88" s="7" t="s">
         <v>304</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_COMP3', </v>
+        <v xml:space="preserve">'NU_NOTA_COMP4', </v>
       </c>
       <c r="B89" s="7" t="s">
         <v>305</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_COMP4', </v>
+        <v>'NU_NOTA_COMP5',</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>306</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>'NU_NOTA_COMP5',</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="C91" s="7"/>
+        <v xml:space="preserve">'NU_NOTA_REDACAO', </v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C91" s="4"/>
       <c r="D91" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">'NU_NOTA_REDACAO', </v>
-      </c>
-      <c r="B92" s="4" t="s">
+      <c r="A92" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C92" s="4"/>
+      <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>296</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>297</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>298</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>299</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>300</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>301</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D100" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G100" s="1" t="s">
+      <c r="G99" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H100" s="1" t="s">
+      <c r="H99" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="1" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>180</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D128" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D129" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="130" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D130" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D131" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D132" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D133" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D134" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D135" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D136" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D137" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D138" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D139" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D140" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D141" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="142" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D142" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D143" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="144" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D144" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="145" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D145" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D146" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D147" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="148" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D148" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="149" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D149" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D150" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="151" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D151" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D152" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="153" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D153" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="154" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D154" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="155" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D155" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D156" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D157" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="158" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D158" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="159" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D159" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="160" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D160" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D161" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D162" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D163" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D164" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>166</v>
+      <c r="D164" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G164" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D165" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D166" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D167" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D168" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D169" s="2" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D170" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D171" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D172" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="str">
+        <f t="shared" ref="A173:A180" si="2">D173</f>
+        <v xml:space="preserve">'TX_RESPOSTAS_CN', </v>
+      </c>
       <c r="D173" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="str">
-        <f t="shared" ref="A174:A181" si="2">D174</f>
-        <v xml:space="preserve">'TX_RESPOSTAS_CN', </v>
+        <f t="shared" si="2"/>
+        <v>'TX_RESPOSTAS_CH',</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>'TX_RESPOSTAS_CH',</v>
+        <v xml:space="preserve">'TX_RESPOSTAS_LC', </v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'TX_RESPOSTAS_LC', </v>
+        <v xml:space="preserve">'TX_RESPOSTAS_MT', </v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'TX_RESPOSTAS_MT', </v>
+        <v xml:space="preserve">'TX_GABARITO_CN', </v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'TX_GABARITO_CN', </v>
+        <v xml:space="preserve">'TX_GABARITO_CH', </v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'TX_GABARITO_CH', </v>
+        <v>'TX_GABARITO_LC',</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>'TX_GABARITO_LC',</v>
+        <v xml:space="preserve">'TX_GABARITO_MT', </v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">'TX_GABARITO_MT', </v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F181" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G181" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H181" s="2" t="s">
-        <v>109</v>
+      <c r="A181" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>142</v>
+        <v>197</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F183" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G183" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H183" s="1" t="s">
-        <v>167</v>
+      <c r="A183" s="1" t="str">
+        <f>D183</f>
+        <v>'CO_MUNICIPIO_RESIDENCIA',</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G183" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H183" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="str">
         <f>D184</f>
-        <v>'CO_MUNICIPIO_RESIDENCIA',</v>
-      </c>
+        <v xml:space="preserve">'CO_MUNICIPIO_NASCIMENTO', </v>
+      </c>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
       <c r="D184" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>3</v>
+        <v>171</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>3</v>
+        <v>171</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>3</v>
+        <v>171</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>3</v>
+        <v>171</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="str">
         <f>D185</f>
-        <v xml:space="preserve">'CO_MUNICIPIO_NASCIMENTO', </v>
-      </c>
-      <c r="B185" s="6"/>
-      <c r="C185" s="6"/>
+        <v>'CO_MUNICIPIO_PROVA',</v>
+      </c>
       <c r="D185" s="2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="str">
-        <f>D186</f>
-        <v>'CO_MUNICIPIO_PROVA',</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H186" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>